<commit_message>
Updated the way of getting the order tracker from Sharepoint using API
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\Group\RPA\Ui Path Code\Alexandra\PRC_Recharges_Performer_VodafoneEquipment\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C4DEA4F-8CE4-402C-8582-96C6544B3069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DD8956-A95D-4175-B815-A0EB80702302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="144">
   <si>
     <t>Name</t>
   </si>
@@ -461,6 +461,15 @@
   </si>
   <si>
     <t>Recharges_SharePoint_TenentID</t>
+  </si>
+  <si>
+    <t>Recharges_VodafoneEquipment_OrderTracker</t>
+  </si>
+  <si>
+    <t>Recharges_VodafoneEquipment_OrderTracker_Subfolder</t>
+  </si>
+  <si>
+    <t>IT Service Delivery Team Site URL</t>
   </si>
 </sst>
 </file>
@@ -856,12 +865,12 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5234375" customWidth="1"/>
+    <col min="1" max="1" width="43.5546875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="81.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2282,12 +2291,12 @@
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.41796875" customWidth="1"/>
-    <col min="4" max="26" width="8.68359375" customWidth="1"/>
+    <col min="3" max="3" width="75.44140625" customWidth="1"/>
+    <col min="4" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2335,7 +2344,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="28.8">
+    <row r="3" spans="1:26" ht="43.2">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -3442,15 +3451,15 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.41796875" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.89453125" customWidth="1"/>
-    <col min="2" max="2" width="30.1015625" customWidth="1"/>
-    <col min="3" max="3" width="60.3125" customWidth="1"/>
-    <col min="4" max="26" width="65.41796875" customWidth="1"/>
+    <col min="1" max="1" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="60.33203125" customWidth="1"/>
+    <col min="4" max="26" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -3548,9 +3557,30 @@
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>142</v>
+      </c>
+      <c r="B10" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+    </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>